<commit_message>
update product template (minor)
</commit_message>
<xml_diff>
--- a/public/product_template.xlsx
+++ b/public/product_template.xlsx
@@ -5,18 +5,18 @@
   <workbookPr dateCompatibility="0" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/william34/Documents/Binus Stuffs/Thesis Stuffs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/william34/Documents/Binus Stuffs/Thesis Stuffs/product-template-stuffs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{724D118B-2352-7148-AE66-A3AF4E4E43D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{250ADAA4-9D05-B24E-AEAD-8E0676483744}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="1320" windowWidth="27640" windowHeight="16680" xr2:uid="{C2AA9022-4DFA-6745-A8D2-A9060B0FD34E}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{C2AA9022-4DFA-6745-A8D2-A9060B0FD34E}"/>
   </bookViews>
   <sheets>
-    <sheet name="product_template (2)" sheetId="2" r:id="rId1"/>
+    <sheet name="product_template" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="ExternalData_1" localSheetId="0" hidden="1">'product_template (2)'!$A$1:$F$2</definedName>
+    <definedName name="ExternalData_1" localSheetId="0" hidden="1">product_template!$A$1:$F$3</definedName>
   </definedNames>
   <calcPr calcId="0"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="9" uniqueCount="9">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="12" uniqueCount="11">
   <si>
     <t>Name</t>
   </si>
@@ -56,13 +56,19 @@
     <t>Quantity</t>
   </si>
   <si>
-    <t>Sample Product</t>
-  </si>
-  <si>
     <t>Sample description</t>
   </si>
   <si>
     <t>Category A</t>
+  </si>
+  <si>
+    <t>Sample Product 1</t>
+  </si>
+  <si>
+    <t>Sample Product 2</t>
+  </si>
+  <si>
+    <t>Category B</t>
   </si>
 </sst>
 </file>
@@ -546,8 +552,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -632,8 +639,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B33D38CC-2D90-B14C-B46B-C37EE06E2BFB}" name="product_template" displayName="product_template" ref="A1:F2" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:F2" xr:uid="{B33D38CC-2D90-B14C-B46B-C37EE06E2BFB}"/>
+<table xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B33D38CC-2D90-B14C-B46B-C37EE06E2BFB}" name="product_template" displayName="product_template" ref="A1:F3" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:F3" xr:uid="{B33D38CC-2D90-B14C-B46B-C37EE06E2BFB}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{59C4B81A-BE93-B644-9251-145CE17D6B94}" uniqueName="1" name="Name" queryTableFieldId="1" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{6101C1A4-96BC-4541-8968-6D77B02B1ED7}" uniqueName="2" name="Description" queryTableFieldId="2" dataDxfId="1"/>
@@ -963,16 +970,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7EA93F1-6145-B34B-93CF-D200DD306B2E}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" customWidth="1"/>
     <col min="3" max="3" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
@@ -1000,13 +1007,13 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
       </c>
       <c r="D2">
         <v>10000</v>
@@ -1016,6 +1023,26 @@
       </c>
       <c r="F2">
         <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3">
+        <v>13000</v>
+      </c>
+      <c r="E3">
+        <v>150000</v>
+      </c>
+      <c r="F3">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>